<commit_message>
checking interference in the pressure sensor data
</commit_message>
<xml_diff>
--- a/RCS Single Stream Test (03-12-2015)/Calibrations.xlsx
+++ b/RCS Single Stream Test (03-12-2015)/Calibrations.xlsx
@@ -662,6 +662,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1000,6 +1001,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -1094,6 +1096,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -1251,6 +1254,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1442,6 +1446,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -1541,6 +1546,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -3311,7 +3317,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="67" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="103" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3322,7 +3328,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="67" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="103" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3676,7 +3682,7 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+      <selection activeCell="A15" sqref="A15:S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
added graphs for data
</commit_message>
<xml_diff>
--- a/RCS Single Stream Test (03-12-2015)/Calibrations.xlsx
+++ b/RCS Single Stream Test (03-12-2015)/Calibrations.xlsx
@@ -11,6 +11,7 @@
     <sheet name="Pressure Calibration" sheetId="2" r:id="rId2"/>
     <sheet name="Force Calibration" sheetId="3" r:id="rId3"/>
     <sheet name="Temperature Calibration" sheetId="4" r:id="rId4"/>
+    <sheet name="Temp calibration (3-10-15)" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -167,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -189,6 +190,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -238,7 +242,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -292,7 +295,7 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.33649469010374183"/>
+                  <c:x val="-0.33649469010374194"/>
                   <c:y val="0.13414603915950304"/>
                 </c:manualLayout>
               </c:layout>
@@ -399,12 +402,560 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="78023680"/>
-        <c:axId val="78029952"/>
+        <c:axId val="157800704"/>
+        <c:axId val="157807744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="78023680"/>
+        <c:axId val="157800704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Raw (V)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="157807744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="157807744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Pressure (psi)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="157800704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Force Calibration</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.4140589009590054E-2"/>
+          <c:y val="7.4850305110299581E-2"/>
+          <c:w val="0.92671841550089595"/>
+          <c:h val="0.8399905357171803"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>3/12/2015</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-7.1574253503943433E-2"/>
+                  <c:y val="6.5520295611058016E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$5:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>4.3052762762762677E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.6944309999999816E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.153113513513512E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5318521521521493E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.2162575575575598E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.7845608608608598E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$6:$G$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.98099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.962</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.9430000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.9239999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.9050000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>3/10/2015</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.6472457669872571E-3"/>
+                  <c:y val="-0.36194954691891196"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$5:$Q$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>-9.4777991967871497E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.100877601609658</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.107250769076305</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.114140096385543</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.266115068273092</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.14189497188754999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$6:$Q$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.98178480000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4730696000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.9430000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19.62</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.8860000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="167729024"/>
+        <c:axId val="174801664"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="167729024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -494,564 +1045,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78029952"/>
+        <c:crossAx val="174801664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="78029952"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Pressure (psi)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="78023680"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Force Calibration</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:title>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="5.4140589009590054E-2"/>
-          <c:y val="7.4850305110299581E-2"/>
-          <c:w val="0.92671841550089584"/>
-          <c:h val="0.83999053571718019"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>3/12/2015</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="5.7635163223310852E-2"/>
-                  <c:y val="-3.7615280399241467E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$5:$G$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>4.3052762762762677E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.6944309999999816E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.153113513513512E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.5318521521521493E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.2162575575575598E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.7845608608608598E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$6:$G$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.98099999999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.962</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.9430000000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.9239999999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.9050000000000002</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>3/10/2015</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-7.3396436698967907E-2"/>
-                  <c:y val="6.9440282059781352E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$L$5:$Q$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>9.4777991967871497E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.100877601609658</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.107250769076305</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.114140096385543</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.266115068273092</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.14189497188754999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$L$6:$Q$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.98178480000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.4730696000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.9430000000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>19.62</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.8860000000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-        </c:ser>
-        <c:dLbls/>
-        <c:axId val="82293120"/>
-        <c:axId val="82295040"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="82293120"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Raw (V)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="82295040"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="82295040"/>
+        <c:axId val="174801664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1141,7 +1140,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82293120"/>
+        <c:crossAx val="167729024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1160,8 +1159,8 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.82371282798749768"/>
-          <c:y val="0.66405863914545604"/>
-          <c:w val="0.15578443994850105"/>
+          <c:y val="0.66405863914545615"/>
+          <c:w val="0.15578443994850108"/>
           <c:h val="5.3479871873060386E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -1309,7 +1308,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="-0.28574743009554299"/>
-                  <c:y val="2.9388854583423787E-2"/>
+                  <c:y val="2.9388854583423794E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1391,12 +1390,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="82579456"/>
-        <c:axId val="82581376"/>
+        <c:axId val="198130688"/>
+        <c:axId val="198157824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="82579456"/>
+        <c:axId val="198130688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1491,12 +1489,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82581376"/>
+        <c:crossAx val="198157824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="82581376"/>
+        <c:axId val="198157824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1591,7 +1589,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82579456"/>
+        <c:crossAx val="198130688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1631,6 +1629,117 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-7.7280120651728693E-2"/>
+                  <c:y val="-6.5495616820193475E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$8:$O$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>-3.7711222444889911E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6322024048096224E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.8396506024096469E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3773599999999974E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$9:$O$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>46</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="156732800"/>
+        <c:axId val="157627520"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="156732800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="157627520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="157627520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="156732800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
 </c:chartSpace>
 </file>
 
@@ -3335,6 +3444,17 @@
 </chartsheet>
 </file>
 
+<file path=xl/chartsheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="103" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
@@ -3394,6 +3514,33 @@
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
     <xdr:ext cx="8672015" cy="6293134"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8674223" cy="6297597"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -3671,7 +3818,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3682,7 +3829,7 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:S21"/>
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3749,6 +3896,12 @@
         <f>ABS(-2.54139673420261)</f>
         <v>2.54139673420261</v>
       </c>
+      <c r="H2" s="9">
+        <v>1333.2</v>
+      </c>
+      <c r="I2" s="10">
+        <v>-1324.2</v>
+      </c>
       <c r="J2" s="3"/>
       <c r="L2" s="1">
         <v>0.99594030999999938</v>
@@ -3791,6 +3944,8 @@
       <c r="G3" s="1">
         <v>2000</v>
       </c>
+      <c r="H3" s="9"/>
+      <c r="I3" s="10"/>
       <c r="J3" s="3"/>
       <c r="L3" s="2">
         <v>0</v>
@@ -3857,28 +4012,34 @@
       </c>
       <c r="J5" s="3"/>
       <c r="L5" s="1">
-        <f>ABS(-0.0947779919678715)</f>
-        <v>9.4777991967871497E-2</v>
+        <f>-0.0947779919678715</f>
+        <v>-9.4777991967871497E-2</v>
       </c>
       <c r="M5" s="1">
-        <f>ABS(-0.100877601609658)</f>
-        <v>0.100877601609658</v>
+        <f>-0.100877601609658</f>
+        <v>-0.100877601609658</v>
       </c>
       <c r="N5" s="1">
-        <f>ABS(-0.107250769076305)</f>
-        <v>0.107250769076305</v>
+        <f>-0.107250769076305</f>
+        <v>-0.107250769076305</v>
       </c>
       <c r="O5" s="1">
-        <f>ABS(-0.114140096385543)</f>
-        <v>0.114140096385543</v>
+        <f>-0.114140096385543</f>
+        <v>-0.114140096385543</v>
       </c>
       <c r="P5" s="1">
-        <f>ABS(-0.266115068273092)</f>
-        <v>0.266115068273092</v>
+        <f>-0.266115068273092</f>
+        <v>-0.266115068273092</v>
       </c>
       <c r="Q5" s="1">
-        <f>ABS(-0.14189497188755)</f>
-        <v>0.14189497188754999</v>
+        <f>-0.14189497188755</f>
+        <v>-0.14189497188754999</v>
+      </c>
+      <c r="R5" s="9">
+        <v>-113.26</v>
+      </c>
+      <c r="S5" s="11">
+        <v>-10.423</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -3934,6 +4095,8 @@
         <f>600*9.81/1000</f>
         <v>5.8860000000000001</v>
       </c>
+      <c r="R6" s="9"/>
+      <c r="S6" s="11"/>
     </row>
     <row r="7" spans="1:20">
       <c r="B7" s="1"/>
@@ -3996,6 +4159,12 @@
       </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
+      <c r="R8" s="9">
+        <v>10804</v>
+      </c>
+      <c r="S8" s="11">
+        <v>28.344999999999999</v>
+      </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
@@ -4034,9 +4203,11 @@
       </c>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="14">
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="L1:Q1"/>
     <mergeCell ref="R2:R3"/>
@@ -4045,6 +4216,12 @@
     <mergeCell ref="H5:H6"/>
     <mergeCell ref="I8:I9"/>
     <mergeCell ref="I5:I6"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="R5:R6"/>
+    <mergeCell ref="S5:S6"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="S8:S9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
single stream data for paper
</commit_message>
<xml_diff>
--- a/RCS Single Stream Test (03-12-2015)/Calibrations.xlsx
+++ b/RCS Single Stream Test (03-12-2015)/Calibrations.xlsx
@@ -168,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -177,6 +177,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -295,7 +298,7 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.33649469010374194"/>
+                  <c:x val="-0.33649469010374206"/>
                   <c:y val="0.13414603915950304"/>
                 </c:manualLayout>
               </c:layout>
@@ -331,7 +334,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>(Sheet1!$B$2:$G$2,Sheet1!$L$2:$N$2)</c:f>
+              <c:f>(Sheet1!$B$2:$G$2,Sheet1!$N$2:$P$2)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -367,7 +370,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(Sheet1!$B$3:$G$3,Sheet1!$L$3:$N$3)</c:f>
+              <c:f>(Sheet1!$B$3:$G$3,Sheet1!$N$3:$P$3)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -402,11 +405,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="157800704"/>
-        <c:axId val="157807744"/>
+        <c:axId val="77044352"/>
+        <c:axId val="77050624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="157800704"/>
+        <c:axId val="77044352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -495,12 +498,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="157807744"/>
+        <c:crossAx val="77050624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="157807744"/>
+        <c:axId val="77050624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -589,7 +592,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="157800704"/>
+        <c:crossAx val="77044352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -662,7 +665,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -679,8 +681,8 @@
           <c:yMode val="edge"/>
           <c:x val="5.4140589009590054E-2"/>
           <c:y val="7.4850305110299581E-2"/>
-          <c:w val="0.92671841550089595"/>
-          <c:h val="0.8399905357171803"/>
+          <c:w val="0.92671841550089606"/>
+          <c:h val="0.83999053571718041"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -898,7 +900,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$L$5:$Q$5</c:f>
+              <c:f>Sheet1!$N$5:$S$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -925,7 +927,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$L$6:$Q$6</c:f>
+              <c:f>Sheet1!$N$6:$S$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -951,11 +953,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="167729024"/>
-        <c:axId val="174801664"/>
+        <c:axId val="77405184"/>
+        <c:axId val="77440128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="167729024"/>
+        <c:axId val="77405184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1000,7 +1002,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -1045,12 +1046,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="174801664"/>
+        <c:crossAx val="77440128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="174801664"/>
+        <c:axId val="77440128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1095,7 +1096,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -1140,7 +1140,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="167729024"/>
+        <c:crossAx val="77405184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1159,8 +1159,8 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.82371282798749768"/>
-          <c:y val="0.66405863914545615"/>
-          <c:w val="0.15578443994850108"/>
+          <c:y val="0.66405863914545626"/>
+          <c:w val="0.15578443994850111"/>
           <c:h val="5.3479871873060386E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -1253,7 +1253,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1308,7 +1307,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="-0.28574743009554299"/>
-                  <c:y val="2.9388854583423794E-2"/>
+                  <c:y val="2.9388854583423798E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1390,11 +1389,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="198130688"/>
-        <c:axId val="198157824"/>
+        <c:axId val="76593408"/>
+        <c:axId val="77869440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="198130688"/>
+        <c:axId val="76593408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1444,7 +1443,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -1489,12 +1487,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="198157824"/>
+        <c:crossAx val="77869440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="198157824"/>
+        <c:axId val="77869440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1544,7 +1542,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -1589,7 +1586,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="198130688"/>
+        <c:crossAx val="76593408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1655,8 +1652,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-7.7280120651728693E-2"/>
-                  <c:y val="-6.5495616820193475E-2"/>
+                  <c:x val="-7.7280120651728706E-2"/>
+                  <c:y val="-6.5495616820193503E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1664,7 +1661,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$L$8:$O$8</c:f>
+              <c:f>Sheet1!$N$8:$Q$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1685,7 +1682,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$L$9:$O$9</c:f>
+              <c:f>Sheet1!$N$9:$Q$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1705,23 +1702,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="156732800"/>
-        <c:axId val="157627520"/>
+        <c:axId val="77910016"/>
+        <c:axId val="77911552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="156732800"/>
+        <c:axId val="77910016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="157627520"/>
+        <c:crossAx val="77911552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="157627520"/>
+        <c:axId val="77911552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1729,14 +1726,13 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="156732800"/>
+        <c:crossAx val="77910016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -3818,7 +3814,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3826,10 +3822,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T9"/>
+  <dimension ref="A1:V9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3837,15 +3833,15 @@
     <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B1" s="6" t="s">
+    <row r="1" spans="1:22" ht="16.5" thickTop="1" thickBot="1">
+      <c r="B1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="9"/>
       <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
@@ -3853,22 +3849,24 @@
         <v>8</v>
       </c>
       <c r="J1" s="4"/>
-      <c r="L1" s="6" t="s">
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="N1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
       <c r="Q1" s="8"/>
-      <c r="R1" t="s">
+      <c r="R1" s="8"/>
+      <c r="S1" s="9"/>
+      <c r="T1" t="s">
         <v>7</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="15.75" thickTop="1">
+    <row r="2" spans="1:22" ht="15.75" thickTop="1">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -3896,33 +3894,35 @@
         <f>ABS(-2.54139673420261)</f>
         <v>2.54139673420261</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2" s="10">
         <v>1333.2</v>
       </c>
-      <c r="I2" s="10">
+      <c r="I2" s="11">
         <v>-1324.2</v>
       </c>
-      <c r="J2" s="3"/>
-      <c r="L2" s="1">
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="3"/>
+      <c r="N2" s="1">
         <v>0.99594030999999938</v>
       </c>
-      <c r="M2" s="1">
+      <c r="O2" s="1">
         <v>1.7703526367265447</v>
       </c>
-      <c r="N2" s="1">
+      <c r="P2" s="1">
         <v>2.4649178483033909</v>
       </c>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
-      <c r="R2" s="9">
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="10">
         <v>1333.2</v>
       </c>
-      <c r="S2" s="10">
+      <c r="U2" s="11">
         <v>-1324.2</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:22">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -3944,28 +3944,30 @@
       <c r="G3" s="1">
         <v>2000</v>
       </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="3"/>
-      <c r="L3" s="2">
+      <c r="H3" s="10"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="3"/>
+      <c r="N3" s="2">
         <v>0</v>
       </c>
-      <c r="M3" s="2">
+      <c r="O3" s="2">
         <v>1000</v>
       </c>
-      <c r="N3" s="2">
+      <c r="P3" s="2">
         <v>2050</v>
       </c>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="10"/>
-      <c r="T3" t="s">
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="11"/>
+      <c r="V3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:22">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -3975,14 +3977,16 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:22">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -4004,45 +4008,47 @@
       <c r="G5" s="1">
         <v>2.7845608608608598E-2</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="10">
         <v>207.56</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="11">
         <v>-0.65600000000000003</v>
       </c>
-      <c r="J5" s="3"/>
-      <c r="L5" s="1">
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="3"/>
+      <c r="N5" s="1">
         <f>-0.0947779919678715</f>
         <v>-9.4777991967871497E-2</v>
       </c>
-      <c r="M5" s="1">
+      <c r="O5" s="1">
         <f>-0.100877601609658</f>
         <v>-0.100877601609658</v>
       </c>
-      <c r="N5" s="1">
+      <c r="P5" s="1">
         <f>-0.107250769076305</f>
         <v>-0.107250769076305</v>
       </c>
-      <c r="O5" s="1">
+      <c r="Q5" s="1">
         <f>-0.114140096385543</f>
         <v>-0.114140096385543</v>
       </c>
-      <c r="P5" s="1">
+      <c r="R5" s="1">
         <f>-0.266115068273092</f>
         <v>-0.266115068273092</v>
       </c>
-      <c r="Q5" s="1">
+      <c r="S5" s="1">
         <f>-0.14189497188755</f>
         <v>-0.14189497188754999</v>
       </c>
-      <c r="R5" s="9">
+      <c r="T5" s="10">
         <v>-113.26</v>
       </c>
-      <c r="S5" s="11">
+      <c r="U5" s="12">
         <v>-10.423</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:22">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -4069,36 +4075,38 @@
         <f>C6*5</f>
         <v>4.9050000000000002</v>
       </c>
-      <c r="H6" s="9"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="3"/>
-      <c r="L6" s="1">
+      <c r="H6" s="10"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="3"/>
+      <c r="N6" s="1">
         <v>0</v>
       </c>
-      <c r="M6" s="1">
+      <c r="O6" s="1">
         <f>100.08*9.81/1000</f>
         <v>0.98178480000000001</v>
       </c>
-      <c r="N6" s="1">
+      <c r="P6" s="1">
         <f>150.16*9.81/1000</f>
         <v>1.4730696000000001</v>
       </c>
-      <c r="O6" s="1">
+      <c r="Q6" s="1">
         <f>300*9.81/1000</f>
         <v>2.9430000000000001</v>
       </c>
-      <c r="P6" s="1">
+      <c r="R6" s="1">
         <f>2000*9.81/1000</f>
         <v>19.62</v>
       </c>
-      <c r="Q6" s="1">
+      <c r="S6" s="1">
         <f>600*9.81/1000</f>
         <v>5.8860000000000001</v>
       </c>
-      <c r="R6" s="9"/>
-      <c r="S6" s="11"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="12"/>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:22">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -4108,14 +4116,16 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:22">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -4135,38 +4145,40 @@
         <v>61.44</v>
       </c>
       <c r="G8" s="1"/>
-      <c r="H8" s="9">
+      <c r="H8" s="10">
         <v>1.2466999999999999</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="11">
         <v>-7.5959000000000003</v>
       </c>
-      <c r="J8" s="3"/>
-      <c r="K8" t="s">
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="3"/>
+      <c r="M8" t="s">
         <v>1</v>
       </c>
-      <c r="L8" s="1">
+      <c r="N8" s="1">
         <v>-3.7711222444889911E-4</v>
       </c>
-      <c r="M8" s="1">
+      <c r="O8" s="1">
         <v>1.6322024048096224E-3</v>
       </c>
-      <c r="N8" s="1">
+      <c r="P8" s="1">
         <v>2.8396506024096469E-3</v>
       </c>
-      <c r="O8" s="1">
+      <c r="Q8" s="1">
         <v>1.3773599999999974E-3</v>
       </c>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="9">
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="10">
         <v>10804</v>
       </c>
-      <c r="S8" s="11">
+      <c r="U8" s="12">
         <v>28.344999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:22">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -4186,42 +4198,44 @@
         <v>69</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="3"/>
-      <c r="L9" s="1">
+      <c r="H9" s="10"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="3"/>
+      <c r="N9" s="1">
         <v>21.5</v>
       </c>
-      <c r="M9" s="1">
+      <c r="O9" s="1">
         <v>50</v>
       </c>
-      <c r="N9" s="1">
+      <c r="P9" s="1">
         <v>55</v>
       </c>
-      <c r="O9" s="1">
+      <c r="Q9" s="1">
         <v>46</v>
       </c>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="9"/>
-      <c r="S9" s="11"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="14">
     <mergeCell ref="B1:G1"/>
-    <mergeCell ref="L1:Q1"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="N1:S1"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="U2:U3"/>
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="H5:H6"/>
     <mergeCell ref="I8:I9"/>
     <mergeCell ref="I5:I6"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="I2:I3"/>
-    <mergeCell ref="R5:R6"/>
-    <mergeCell ref="S5:S6"/>
-    <mergeCell ref="R8:R9"/>
-    <mergeCell ref="S8:S9"/>
+    <mergeCell ref="T5:T6"/>
+    <mergeCell ref="U5:U6"/>
+    <mergeCell ref="T8:T9"/>
+    <mergeCell ref="U8:U9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>